<commit_message>
updated Sample Data For User Entity.xlsx
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
+++ b/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
@@ -5,27 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Documents\Gdp-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D22FCD-6ADE-4033-AC05-2DDA6DB395F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA545D6-43DD-4E31-AF16-23FB11F25992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>Username</t>
   </si>
@@ -100,6 +108,45 @@
   </si>
   <si>
     <t>Sowmya</t>
+  </si>
+  <si>
+    <t>Curie</t>
+  </si>
+  <si>
+    <t>Daley</t>
+  </si>
+  <si>
+    <t>Dali</t>
+  </si>
+  <si>
+    <t>Dali547</t>
+  </si>
+  <si>
+    <t>Daley547</t>
+  </si>
+  <si>
+    <t>Curie547</t>
+  </si>
+  <si>
+    <t>Dali@gmail.com</t>
+  </si>
+  <si>
+    <t>Daley@gmail.com</t>
+  </si>
+  <si>
+    <t>Curie@gmail.com</t>
+  </si>
+  <si>
+    <t>Gary</t>
+  </si>
+  <si>
+    <t>Gary@gmail.com</t>
+  </si>
+  <si>
+    <t>Emilysmith</t>
+  </si>
+  <si>
+    <t>emily@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -152,11 +199,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -438,17 +491,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="3" max="3" width="23.36328125" customWidth="1"/>
     <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -652,6 +705,109 @@
       <c r="F10" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3">
+        <v>44075</v>
+      </c>
+      <c r="E11" s="3">
+        <v>44083</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3">
+        <v>44075</v>
+      </c>
+      <c r="E12" s="3">
+        <v>44083</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3">
+        <v>44075</v>
+      </c>
+      <c r="E13" s="3">
+        <v>44083</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="3">
+        <v>44075</v>
+      </c>
+      <c r="E14" s="3">
+        <v>44083</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="3">
+        <v>44075</v>
+      </c>
+      <c r="E15" s="3">
+        <v>44083</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -664,8 +820,13 @@
     <hyperlink ref="C8" r:id="rId7" xr:uid="{D7C97792-0AB2-4AC9-AC13-3D165379A529}"/>
     <hyperlink ref="C9" r:id="rId8" xr:uid="{1555F725-C14F-4D57-AEE7-7A123C8E139C}"/>
     <hyperlink ref="C10" r:id="rId9" xr:uid="{0ACB9200-A25A-40EE-B246-3616FA66BEAE}"/>
+    <hyperlink ref="C13" r:id="rId10" xr:uid="{4795649A-066C-434A-9B92-8E017F070716}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{3A6789BE-4043-49F8-B245-2CE3772121AF}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{8B29F0E4-2189-4C21-9644-C3B5028895E5}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{7C2F7A01-A2F2-407A-B950-C1990ECEB96D}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{17F24917-A2D8-4FE8-AA86-0399A53A03D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Water intake in Sample Data For User Entity.xlsx
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
+++ b/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99019CB-43C6-4107-A018-90926057B9B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B6BC2C-07F4-470B-AFAB-49788261817C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Entity" sheetId="1" r:id="rId1"/>
+    <sheet name="Water Intake" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="55">
   <si>
     <t>Username</t>
   </si>
@@ -138,13 +139,73 @@
   </si>
   <si>
     <t>emily@gmail.com</t>
+  </si>
+  <si>
+    <t>Water Intake(1 gallon/3.78 liters)</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>3 liters</t>
+  </si>
+  <si>
+    <t>3.5 liters</t>
+  </si>
+  <si>
+    <t>1.2 gallon</t>
+  </si>
+  <si>
+    <t>0.9 gallon</t>
+  </si>
+  <si>
+    <t>4 liters</t>
+  </si>
+  <si>
+    <t>2.9 liters</t>
+  </si>
+  <si>
+    <t>0.95 gallons</t>
+  </si>
+  <si>
+    <t>3.7 liters</t>
+  </si>
+  <si>
+    <t>1.1 gallon</t>
+  </si>
+  <si>
+    <t>1 gallon</t>
+  </si>
+  <si>
+    <t>1.5 gallon</t>
+  </si>
+  <si>
+    <t>3.1 liters</t>
+  </si>
+  <si>
+    <t>5 liters</t>
+  </si>
+  <si>
+    <t>3.6 liters</t>
+  </si>
+  <si>
+    <t>0.95 gallon</t>
+  </si>
+  <si>
+    <t>1.3 gallon</t>
+  </si>
+  <si>
+    <t>0.8 gallon</t>
+  </si>
+  <si>
+    <t>0.85 gallon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +225,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,7 +257,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -200,6 +267,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -484,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -820,4 +891,860 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952D8A45-6F5D-45C7-8CE6-813C640B842B}">
+  <dimension ref="A1:Q16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+    <col min="6" max="7" width="9.81640625" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" customWidth="1"/>
+    <col min="11" max="11" width="10.7265625" customWidth="1"/>
+    <col min="12" max="12" width="10.26953125" customWidth="1"/>
+    <col min="13" max="13" width="10.36328125" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="15" max="15" width="10.36328125" customWidth="1"/>
+    <col min="16" max="16" width="9.7265625" customWidth="1"/>
+    <col min="17" max="17" width="10.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="6">
+        <v>44075</v>
+      </c>
+      <c r="C2" s="6">
+        <v>44076</v>
+      </c>
+      <c r="D2" s="6">
+        <v>44077</v>
+      </c>
+      <c r="E2" s="6">
+        <v>44078</v>
+      </c>
+      <c r="F2" s="6">
+        <v>44079</v>
+      </c>
+      <c r="G2" s="6">
+        <v>44080</v>
+      </c>
+      <c r="H2" s="6">
+        <v>44081</v>
+      </c>
+      <c r="I2" s="6">
+        <v>44082</v>
+      </c>
+      <c r="J2" s="6">
+        <v>44083</v>
+      </c>
+      <c r="K2" s="6">
+        <v>44084</v>
+      </c>
+      <c r="L2" s="6">
+        <v>44085</v>
+      </c>
+      <c r="M2" s="6">
+        <v>44086</v>
+      </c>
+      <c r="N2" s="6">
+        <v>44087</v>
+      </c>
+      <c r="O2" s="6">
+        <v>44088</v>
+      </c>
+      <c r="P2" s="6">
+        <v>44089</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>44090</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P9" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" t="s">
+        <v>48</v>
+      </c>
+      <c r="P10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" t="s">
+        <v>51</v>
+      </c>
+      <c r="P13" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" t="s">
+        <v>51</v>
+      </c>
+      <c r="M14" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" t="s">
+        <v>51</v>
+      </c>
+      <c r="M15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O15" t="s">
+        <v>45</v>
+      </c>
+      <c r="P15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" t="s">
+        <v>44</v>
+      </c>
+      <c r="N16" t="s">
+        <v>44</v>
+      </c>
+      <c r="O16" t="s">
+        <v>44</v>
+      </c>
+      <c r="P16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A16">
+    <sortCondition ref="A3"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated user in Sample Data For User Entity.xlsx
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
+++ b/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADECE274-D2E4-4897-B318-B0AAA246E43D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ED2B06-230A-4B2C-9C38-087CF90BAE15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Username</t>
   </si>
@@ -141,6 +141,30 @@
   </si>
   <si>
     <t>User ID</t>
+  </si>
+  <si>
+    <t>johnsmith99</t>
+  </si>
+  <si>
+    <t>amyjackson</t>
+  </si>
+  <si>
+    <t>sophiacathie</t>
+  </si>
+  <si>
+    <t>jacobmason</t>
+  </si>
+  <si>
+    <t>emmawilliam</t>
+  </si>
+  <si>
+    <t>Oliviajaden</t>
+  </si>
+  <si>
+    <t>Natasha99</t>
+  </si>
+  <si>
+    <t>danieldanny</t>
   </si>
 </sst>
 </file>
@@ -503,7 +527,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -543,7 +569,7 @@
         <v>222</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -566,7 +592,7 @@
         <v>223</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -589,7 +615,7 @@
         <v>224</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -612,7 +638,7 @@
         <v>225</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -635,7 +661,7 @@
         <v>226</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -658,7 +684,7 @@
         <v>227</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
@@ -681,7 +707,7 @@
         <v>228</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
@@ -704,7 +730,7 @@
         <v>229</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>13</v>
@@ -727,7 +753,7 @@
         <v>230</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>14</v>
@@ -750,7 +776,7 @@
         <v>231</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>25</v>
@@ -866,20 +892,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{38E5C388-79FF-48B3-A7E3-51C74B4B1417}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{C6321951-576B-4BF5-8C39-0F7BF2A9201A}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{5C1045F0-3F93-4668-B0D1-24D69292B631}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{AD89C636-F726-4596-804D-7CCA528B78F1}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{3F45E56F-DFFF-4E60-AA4E-FFFF6BFDA5AA}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{41A56BA4-4D96-414D-A13B-0B44DF04C6BD}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{D7C97792-0AB2-4AC9-AC13-3D165379A529}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{1555F725-C14F-4D57-AEE7-7A123C8E139C}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{0ACB9200-A25A-40EE-B246-3616FA66BEAE}"/>
-    <hyperlink ref="D13" r:id="rId10" xr:uid="{4795649A-066C-434A-9B92-8E017F070716}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{3A6789BE-4043-49F8-B245-2CE3772121AF}"/>
-    <hyperlink ref="D11" r:id="rId12" xr:uid="{8B29F0E4-2189-4C21-9644-C3B5028895E5}"/>
-    <hyperlink ref="D14" r:id="rId13" xr:uid="{7C2F7A01-A2F2-407A-B950-C1990ECEB96D}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{17F24917-A2D8-4FE8-AA86-0399A53A03D0}"/>
+    <hyperlink ref="D13" r:id="rId1" xr:uid="{4795649A-066C-434A-9B92-8E017F070716}"/>
+    <hyperlink ref="D12" r:id="rId2" xr:uid="{3A6789BE-4043-49F8-B245-2CE3772121AF}"/>
+    <hyperlink ref="D14" r:id="rId3" xr:uid="{7C2F7A01-A2F2-407A-B950-C1990ECEB96D}"/>
+    <hyperlink ref="D15" r:id="rId4" xr:uid="{17F24917-A2D8-4FE8-AA86-0399A53A03D0}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{8B29F0E4-2189-4C21-9644-C3B5028895E5}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{0ACB9200-A25A-40EE-B246-3616FA66BEAE}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{1555F725-C14F-4D57-AEE7-7A123C8E139C}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{D7C97792-0AB2-4AC9-AC13-3D165379A529}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{41A56BA4-4D96-414D-A13B-0B44DF04C6BD}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{3F45E56F-DFFF-4E60-AA4E-FFFF6BFDA5AA}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{AD89C636-F726-4596-804D-7CCA528B78F1}"/>
+    <hyperlink ref="D4" r:id="rId12" xr:uid="{5C1045F0-3F93-4668-B0D1-24D69292B631}"/>
+    <hyperlink ref="D3" r:id="rId13" xr:uid="{C6321951-576B-4BF5-8C39-0F7BF2A9201A}"/>
+    <hyperlink ref="D2" r:id="rId14" xr:uid="{38E5C388-79FF-48B3-A7E3-51C74B4B1417}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>

</xml_diff>

<commit_message>
updated email in Sample Data For User Entity.xlsx
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
+++ b/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ED2B06-230A-4B2C-9C38-087CF90BAE15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201D3E92-8C3C-450B-A614-ED82269A1B52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,33 +80,6 @@
     <t>Joseph</t>
   </si>
   <si>
-    <t>Bob@gmail.com</t>
-  </si>
-  <si>
-    <t>James@gmail.com</t>
-  </si>
-  <si>
-    <t>Robert@gmail.com</t>
-  </si>
-  <si>
-    <t>michael@gmail.com</t>
-  </si>
-  <si>
-    <t>william@gmail.com</t>
-  </si>
-  <si>
-    <t>david@gmail.com</t>
-  </si>
-  <si>
-    <t>richard@gmail.com</t>
-  </si>
-  <si>
-    <t>thomas@gmail.com</t>
-  </si>
-  <si>
-    <t>Joseph@gmail.com</t>
-  </si>
-  <si>
     <t>Sowmya</t>
   </si>
   <si>
@@ -125,9 +98,6 @@
     <t>Daley@gmail.com</t>
   </si>
   <si>
-    <t>Curie@gmail.com</t>
-  </si>
-  <si>
     <t>Gary</t>
   </si>
   <si>
@@ -165,6 +135,36 @@
   </si>
   <si>
     <t>danieldanny</t>
+  </si>
+  <si>
+    <t>johnsmith99@gmail.com</t>
+  </si>
+  <si>
+    <t>amyjackson@gmail.com</t>
+  </si>
+  <si>
+    <t>jadewilliam@gmail.com</t>
+  </si>
+  <si>
+    <t>cathiecat@gmail.com</t>
+  </si>
+  <si>
+    <t>mysonjacob@gmail.com</t>
+  </si>
+  <si>
+    <t>willy9898@gmail.com</t>
+  </si>
+  <si>
+    <t>jadejady@gmail.com</t>
+  </si>
+  <si>
+    <t>smartemily@gmail.com</t>
+  </si>
+  <si>
+    <t>naughtynatasha@gmail.com</t>
+  </si>
+  <si>
+    <t>danieldanny77@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,14 +536,14 @@
     <col min="1" max="1" width="8.81640625" customWidth="1"/>
     <col min="2" max="2" width="11.7265625" customWidth="1"/>
     <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" customWidth="1"/>
+    <col min="4" max="4" width="24.54296875" customWidth="1"/>
     <col min="5" max="5" width="11.08984375" customWidth="1"/>
     <col min="6" max="6" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -569,13 +569,13 @@
         <v>222</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E2" s="7">
         <v>44075</v>
@@ -584,7 +584,7 @@
         <v>44083</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -592,13 +592,13 @@
         <v>223</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E3" s="7">
         <v>44075</v>
@@ -607,7 +607,7 @@
         <v>44083</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -621,7 +621,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E4" s="7">
         <v>44075</v>
@@ -630,7 +630,7 @@
         <v>44083</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -638,13 +638,13 @@
         <v>225</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E5" s="7">
         <v>44075</v>
@@ -653,7 +653,7 @@
         <v>44083</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -661,13 +661,13 @@
         <v>226</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="E6" s="7">
         <v>44075</v>
@@ -676,7 +676,7 @@
         <v>44083</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -684,13 +684,13 @@
         <v>227</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E7" s="7">
         <v>44075</v>
@@ -699,7 +699,7 @@
         <v>44083</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -707,13 +707,13 @@
         <v>228</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E8" s="7">
         <v>44075</v>
@@ -722,7 +722,7 @@
         <v>44083</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -730,13 +730,13 @@
         <v>229</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E9" s="7">
         <v>44075</v>
@@ -745,7 +745,7 @@
         <v>44083</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -753,13 +753,13 @@
         <v>230</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E10" s="7">
         <v>44075</v>
@@ -768,7 +768,7 @@
         <v>44083</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -776,14 +776,14 @@
         <v>231</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="E11" s="7">
         <v>44075</v>
       </c>
@@ -791,7 +791,7 @@
         <v>44083</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -799,13 +799,13 @@
         <v>232</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E12" s="7">
         <v>44075</v>
@@ -814,7 +814,7 @@
         <v>44083</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -822,13 +822,13 @@
         <v>233</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E13" s="7">
         <v>44075</v>
@@ -837,7 +837,7 @@
         <v>44083</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -845,13 +845,13 @@
         <v>234</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E14" s="7">
         <v>44075</v>
@@ -860,7 +860,7 @@
         <v>44083</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -868,13 +868,13 @@
         <v>235</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E15" s="7">
         <v>44075</v>
@@ -883,7 +883,7 @@
         <v>44083</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -896,16 +896,16 @@
     <hyperlink ref="D12" r:id="rId2" xr:uid="{3A6789BE-4043-49F8-B245-2CE3772121AF}"/>
     <hyperlink ref="D14" r:id="rId3" xr:uid="{7C2F7A01-A2F2-407A-B950-C1990ECEB96D}"/>
     <hyperlink ref="D15" r:id="rId4" xr:uid="{17F24917-A2D8-4FE8-AA86-0399A53A03D0}"/>
-    <hyperlink ref="D11" r:id="rId5" xr:uid="{8B29F0E4-2189-4C21-9644-C3B5028895E5}"/>
-    <hyperlink ref="D10" r:id="rId6" xr:uid="{0ACB9200-A25A-40EE-B246-3616FA66BEAE}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{1555F725-C14F-4D57-AEE7-7A123C8E139C}"/>
-    <hyperlink ref="D8" r:id="rId8" xr:uid="{D7C97792-0AB2-4AC9-AC13-3D165379A529}"/>
-    <hyperlink ref="D7" r:id="rId9" xr:uid="{41A56BA4-4D96-414D-A13B-0B44DF04C6BD}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{3F45E56F-DFFF-4E60-AA4E-FFFF6BFDA5AA}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{AD89C636-F726-4596-804D-7CCA528B78F1}"/>
-    <hyperlink ref="D4" r:id="rId12" xr:uid="{5C1045F0-3F93-4668-B0D1-24D69292B631}"/>
-    <hyperlink ref="D3" r:id="rId13" xr:uid="{C6321951-576B-4BF5-8C39-0F7BF2A9201A}"/>
-    <hyperlink ref="D2" r:id="rId14" xr:uid="{38E5C388-79FF-48B3-A7E3-51C74B4B1417}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{2C0750FF-F9C0-44E1-B65D-266242274803}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{71E04E96-422C-48E4-BE65-1F1D0659A462}"/>
+    <hyperlink ref="D4" r:id="rId7" xr:uid="{B11BCA15-E726-4769-9CC5-436E54E2540C}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{2C71F906-94C4-4DC4-9D45-CCB6C216D8B4}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{B6FD7640-4DAC-4A83-9FD4-80A539D210D3}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{03A30E57-B935-4658-A2B6-7068A6A697EA}"/>
+    <hyperlink ref="D8" r:id="rId11" xr:uid="{0B0C7D86-5267-481B-85C0-9C1C2BC9E285}"/>
+    <hyperlink ref="D9" r:id="rId12" xr:uid="{9C76E509-D696-4084-986C-C7E68F8F27B6}"/>
+    <hyperlink ref="D11" r:id="rId13" xr:uid="{4F95C6EB-1ACB-4FA5-B459-DF5807175688}"/>
+    <hyperlink ref="D10" r:id="rId14" xr:uid="{C82BCE09-D143-4666-BB4B-3623C2E2B64A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>

</xml_diff>

<commit_message>
Updated admin in Sample Data For User Entity.xlsx
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
+++ b/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201D3E92-8C3C-450B-A614-ED82269A1B52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D87A9AE-17B1-4D85-ADC3-80D82A8D0CC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Username</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Joseph</t>
   </si>
   <si>
-    <t>Sowmya</t>
-  </si>
-  <si>
     <t>Curie</t>
   </si>
   <si>
@@ -165,6 +162,12 @@
   </si>
   <si>
     <t>danieldanny77@gmail.com</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -528,7 +531,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,7 +546,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -569,13 +572,13 @@
         <v>222</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="7">
         <v>44075</v>
@@ -584,7 +587,7 @@
         <v>44083</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -592,13 +595,13 @@
         <v>223</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="7">
         <v>44075</v>
@@ -607,7 +610,7 @@
         <v>44083</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -621,7 +624,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="7">
         <v>44075</v>
@@ -630,7 +633,7 @@
         <v>44083</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -638,13 +641,13 @@
         <v>225</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="7">
         <v>44075</v>
@@ -653,7 +656,7 @@
         <v>44083</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -661,13 +664,13 @@
         <v>226</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="7">
         <v>44075</v>
@@ -676,7 +679,7 @@
         <v>44083</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -684,13 +687,13 @@
         <v>227</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="7">
         <v>44075</v>
@@ -699,7 +702,7 @@
         <v>44083</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -707,13 +710,13 @@
         <v>228</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="7">
         <v>44075</v>
@@ -722,7 +725,7 @@
         <v>44083</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -730,13 +733,13 @@
         <v>229</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="7">
         <v>44075</v>
@@ -745,7 +748,7 @@
         <v>44083</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -753,13 +756,13 @@
         <v>230</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="7">
         <v>44075</v>
@@ -768,7 +771,7 @@
         <v>44083</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -776,13 +779,13 @@
         <v>231</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="7">
         <v>44075</v>
@@ -791,7 +794,7 @@
         <v>44083</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -799,13 +802,13 @@
         <v>232</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="7">
         <v>44075</v>
@@ -814,7 +817,7 @@
         <v>44083</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -822,14 +825,14 @@
         <v>233</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="E13" s="7">
         <v>44075</v>
       </c>
@@ -837,7 +840,7 @@
         <v>44083</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -845,14 +848,14 @@
         <v>234</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="E14" s="7">
         <v>44075</v>
       </c>
@@ -860,7 +863,7 @@
         <v>44083</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -868,14 +871,14 @@
         <v>235</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="E15" s="7">
         <v>44075</v>
       </c>
@@ -883,7 +886,7 @@
         <v>44083</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
made changes to admin and last accessed date
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
+++ b/Design Data/Sample Data/Excel Files/Sample Data For User Entity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Desktop\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD66F05-E289-4EE6-8457-383E8147104F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666BDF02-51BE-4B8C-A300-089EAA7D4457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,7 +525,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,7 +572,7 @@
         <v>44075</v>
       </c>
       <c r="E2" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>42</v>
@@ -592,7 +592,7 @@
         <v>44075</v>
       </c>
       <c r="E3" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>42</v>
@@ -612,7 +612,7 @@
         <v>44075</v>
       </c>
       <c r="E4" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>42</v>
@@ -632,7 +632,7 @@
         <v>44075</v>
       </c>
       <c r="E5" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>43</v>
@@ -652,7 +652,7 @@
         <v>44075</v>
       </c>
       <c r="E6" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>42</v>
@@ -672,7 +672,7 @@
         <v>44075</v>
       </c>
       <c r="E7" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>42</v>
@@ -692,7 +692,7 @@
         <v>44075</v>
       </c>
       <c r="E8" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>42</v>
@@ -712,7 +712,7 @@
         <v>44075</v>
       </c>
       <c r="E9" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>43</v>
@@ -732,7 +732,7 @@
         <v>44075</v>
       </c>
       <c r="E10" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>42</v>
@@ -752,7 +752,7 @@
         <v>44075</v>
       </c>
       <c r="E11" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>42</v>
@@ -772,7 +772,7 @@
         <v>44075</v>
       </c>
       <c r="E12" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>42</v>
@@ -792,7 +792,7 @@
         <v>44075</v>
       </c>
       <c r="E13" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>42</v>
@@ -812,7 +812,7 @@
         <v>44075</v>
       </c>
       <c r="E14" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>42</v>
@@ -832,7 +832,7 @@
         <v>44075</v>
       </c>
       <c r="E15" s="6">
-        <v>44083</v>
+        <v>44091</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>42</v>

</xml_diff>